<commit_message>
Performance improvements & extra examples
</commit_message>
<xml_diff>
--- a/examples/Australia OGD/coloured labour/profile.xlsx
+++ b/examples/Australia OGD/coloured labour/profile.xlsx
@@ -345,7 +345,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,20 +435,30 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
+          <t>default_count</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>default_value</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
           <t>most_frequent_value</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>memory_consumed_bytes</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>pattern_count</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>patterns</t>
         </is>
@@ -508,18 +517,26 @@
       <c r="P2" t="n">
         <v>4</v>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
         <is>
           <t>n/a</t>
         </is>
       </c>
-      <c r="R2" t="n">
+      <c r="T2" t="n">
         <v>22825</v>
       </c>
-      <c r="S2" t="n">
+      <c r="U2" t="n">
         <v>2299</v>
       </c>
-      <c r="T2" t="inlineStr">
+      <c r="V2" t="inlineStr">
         <is>
           <t>['73', 'A SAM', 'ABAS KHAN', 'ABDOOL HOSSAIN', 'ABDUL KARIM', 'ABDUL REZACK', 'ABDULLA', 'ABDULLAH', 'ABLEN', 'ABOOD', 'ABOUD', 'ABRAHAM', 'ABUD', 'ABYAKE', 'ABYSS MULLAH', 'ADALAT KHAN', 'ADDO', 'AGNES', 'AH BACK', 'AH BANG', 'AH BEW', 'AH BING', 'AH BONG', 'AH BOO', 'AH BOW', 'AH BOY', 'AH BUE', 'AH BUN', 'AH BUN LONG', 'AH BUNG', 'AH CHAN', 'AH CHAY', 'AH CHEE', 'AH CHEU', 'AH CHEW', 'AH CHIN', 'AH CHING', 'AH CHIT', 'AH CHONG', 'AH CHOO', 'AH CHOOK', 'AH CHOW', 'AH CHOY', 'AH CHUCK', 'AH CHUE', 'AH CHUM', 'AH CHUNG', 'AH CIER', 'AH CON', 'AH CONG', 'AH CONG ?', 'AH COON', 'AH COW', 'AH COWM', 'AH COY', 'AH DANG', 'AH DAY', 'AH DICK', 'AH DING', 'AH DOCK', 'AH DOEY', 'AH DON', 'AH DONG', 'AH DOO', 'AH DOW', 'AH DOY', 'AH DUCK', 'AH DUNG', 'AH FAH', 'AH FAK', 'AH FAT', 'AH FAY', 'AH FEE', 'AH FONG', 'AH FOO', 'AH FOOK', 'AH FUE', 'AH FUN', 'AH GAB', 'AH GAH', 'AH GEE', 'AH GEO', 'AH GIN', 'AH GING', 'AH GONG', 'AH GOON', 'AH GOW', 'AH GOWM', 'AH GUAY', 'AH GUM', 'AH GUN', 'AH GUY', 'AH HAT', 'AH HAUK', 'AH HAY', 'AH HEE', 'AH HEN', 'AH HIM', 'AH HIN', 'AH HING', 'AH HIP', 'AH HOE', 'AH HOM', 'AH HON', 'AH HONG', 'AH HOO', 'AH HOOK', 'AH HOON', 'AH HOP', 'AH HOW', 'AH HOY', 'AH HUNG', 'AH ING', 'AH JIM', 'AH JOY', 'AH KAN', 'AH KAY', 'AH KEE', 'AH KEN', 'AH KEW', 'AH KIM', 'AH KIN', 'AH KING', 'AH KONG', 'AH KOO', 'AH KOPP', 'AH KOW', 'AH KROI', 'AH LAMAN', 'AH LAY', 'AH LEE', 'AH LEON', 'AH LEONG', 'AH LIC', 'AH LIM', 'AH LIN', 'AH LING', 'AH LIU', 'AH LO', 'AH LOCK', 'AH LOIN', 'AH LONG', 'AH LOO', 'AH LOOEY', 'AH LOOK', 'AH LOONG', 'AH LOP', 'AH LOU', 'AH LOW', 'AH LOY', 'AH LUM', 'AH LUN', 'AH MACK', 'AH MAN', 'AH MAT', 'AH MEE', 'AH MIN', 'AH MON', 'AH MONG', 'AH MOOK', 'AH MOON', 'AH MOONG', 'AH MOW', 'AH MOY', 'AH MUN', 'AH NANG', 'AH NEU?F', 'AH NIM', 'AH NIN', 'AH NU', 'AH NUM', 'AH ON', 'AH ONE', 'AH OUY', 'AH PEN', 'AH PIE', 'AH PIM', 'AH PIN', 'AH PING', 'AH PO', 'AH PONG', 'AH POOEH', 'AH POYE', 'AH QUA', 'AH QUAY', 'AH QUE', 'AH QUINE', 'AH QUIVEN', 'AH QUON', 'AH QUONG', 'AH SAM', 'AH SAME', 'AH SANG', 'AH SAW', 'AH SAY', 'AH SEE', 'AH SEE WAH', 'AH SHANG', 'AH SHIN', 'AH SHING', 'AH SIN', 'AH SING', 'AH SON', 'AH SONG', 'AH SONNG', 'AH SOON', 'AH SOW', 'AH SUE', 'AH SUEY', 'AH SUM', 'AH SUN', 'AH SUNG', 'AH TEE', 'AH TIE', 'AH TIM', 'AH TIN', 'AH TONG', 'AH TOO', 'AH TOON', 'AH TOUNG', 'AH VIM', 'AH WAH', 'AH WAN', 'AH WAR', 'AH WAY', 'AH WEE', 'AH WHY', 'AH WING', 'AH WOAH', 'AH WOE', 'AH WOH', 'AH WON', 'AH WONG', 'AH WOOD', 'AH YACK', 'AH YAT', 'AH YEE', 'AH YEN', 'AH YET', 'AH YEUNN', 'AH YEW', 'AH YICK', 'AH YIN', 'AH YIP', 'AH YOKE', 'AH YONG', 'AH YORK', 'AH YOU', 'AH YOUNG', 'AH YOW', 'AH YOY', 'AH YUM', 'AH YUN', 'AHCOMINIE', 'AHKIE', 'AHLING', 'AHSAN', 'ALACK', 'ALBERT', 'ALEAN', 'ALEC HOP', 'ALI HOOSAN', 'ALICK', 'ALICK MALICOOLA', 'ALICK MATTHEW', 'ALICK NAGUES', 'ALICKEY', 'ALLEY SARA', 'ALLIE', 'ALLUM KHAN', 'AMANAS', 'AMAT', 'AMAUT', 'AMBRUM', 'AMEYTOO', 'AMMOTT', 'AMOLIES', 'AMYRIA', 'ANAMBOON', 'ANDRONICOS', 'ANG GEE', 'ANISOLA', 'ANN JABOOR', 'ANNENPHONE', 'ANTON', 'ANTONI', 'AOSANO', 'APILIS', 'APPOO', 'ARAMANGO', 'ARMANDO', 'ARMAT', 'ARMSTRONG', 'ARRATAGONI', 'ARROW', 'ARRUFA J.WILSON', 'ASASUKE OKI', 'ASCOL', 'ASHIMURA', 'ASTOON', 'ATHIEGHEE', 'ATRES', 'ATTRA', 'AUGUST', 'AVE', 'AYOR', 'BADHR KHAN', 'BAGGOW', 'BALLAD ALLA', 'BALLY', 'BANDIS', 'BANJI', 'BANNY', 'BARACONE', 'BARACOOLA', 'BARCOU', 'BARCOW', 'BARGALLIE', 'BARLOW', 'BARWICK', 'BARY', 'BASCAL', 'BASSER', 'BASSIDIN', 'BATCHE', 'BAXTER', 'BAY FOON', 'BAYOON', 'BEA', 'BEE HANG', 'BEHRAN', 'BERGO', 'BERRA', 'BERRY', 'BEUTLAN', 'BICKY', 'BIEN', 'BIMMINIS', 'BIN LUNG', 'BING CHEW', 'BING FAT', 'BINSAP', 'BOB', 'BOBA', 'BOBETTI', 'BOHAR', 'BOLOUS', 'BOLOW', 'BOMBAY', 'BONG', 'BOOKHE', 'BOOT', 'BOOTER', 'BOSIE', 'BOSLAM', 'BOUGRESS', 'BOW', 'BOW GEE', 'BOW SUN', 'BOWEN', 'BOY', 'BOY JUAN', 'BRAMLOW', 'BRANG', 'BROWMASSING', 'BROWN', 'BUCCA BUCCA', 'BUCH CHUN', 'BUDU', 'BUE', 'BUKAN', 'BULLA', 'BUNG', 'BUNGMEALL', 'BURRA', 'BUT LUN', 'BUTTER', 'CACA', 'CACA HC.', 'CAH CHONG', 'CAH MAT', 'CAISA', 'CALLAPUT', 'CALLAYSEE', 'CAN KONG', 'CANDY', 'CANTONG', 'CARABBA', 'CARDIER', 'CAREEDY', 'CARSSONALLEY', 'CARTO', 'CASEY', 'CASSAM', 'CASSAM JACKSAM', 'CASSELL', 'CEAZAR GORMANS', 'CHAN', 'CHAN BOW', 'CHAN CHONG', 'CHAN HOOK', 'CHANG FEE', 'CHANG FU', 'CHANG SEE', 'CHANG SING', 'CHANG SU', 'CHANG YAK', 'CHANG YIN', 'CHARLIE', 'CHARLIE JOES', 'CHEE GO', 'CHEE QUIN', 'CHEE WAH', 'CHEN HENG', 'CHEN KEN', 'CHEW', 'CHEW BONG', 'CHEW CHONG', 'CHEW FOEY', 'CHEW GUN', 'CHEW KUM', 'CHI QUNN', 'CHIKAZAWA', 'CHIM YOW', 'CHIN', 'CHIN AH COY', 'CHIN CHOW', 'CHIN DI', 'CHIN FOY', 'CHIN HAW', 'CHIN HIN', 'CHIN HOY', 'CHIN JOY', 'CHIN LAI', 'CHIN ON', 'CHIN PAK', 'CHIN SING', 'CHIN WON', 'CHIN YEE', 'CHIN YIPP FOO', 'CHIN YOW', 'CHING', 'CHING DO', 'CHING FAY', 'CHING GOW', 'CHING SHIN', 'CHING WHY', 'CHIORO', 'CHIP MING', 'CHIU CHOW', 'CHIU LOOK', 'CHO CHOY', 'CHON CHAN', 'CHONG', 'CHONG BACK', 'CHONG FOO', 'CHONG GEE', 'CHONG GUM', 'CHONG HOON', 'CHONG KEE', 'CHONG LEE GOW', 'CHONG LOCK', 'CHONG MONG', 'CHONG MOW', 'CHONG PARR', 'CHONG QUAY', 'CHONG SANG', 'CHONG SING', 'CHONG TAI', 'CHONG WAH', 'CHONG WAY', 'CHONG YONG', 'CHOP HING', 'CHOPPY', 'CHOSAKU FURUTA', 'CHOU FOOK', 'CHOU FOOK YIN', 'CHOU FOOK YIU', 'CHOW', 'CHOW FOOK', 'CHOW MUM', 'CHOY', 'CHOY FOUR', 'CHOY GAY', 'CHOY GUM', 'CHOY HOW', 'CHOY JIM', 'CHOY LOOK', 'CHOY QUIN', 'CHOY SHUCK LIN', 'CHOY SING', 'CHOY SUN NARM', 'CHOY YET', 'CHOY YOU', 'CHOY YOW', 'CHUI LOOK', 'CHUICHI NAGOI', 'CHUM CUM MING', 'CHUM HO', 'CHUM KIN', 'CHUN BUE', 'CHUN FOO', 'CHUN FUNG', 'CHUN KEET', 'CHUN PIE', 'CHUN WAH YEE', 'CHUN YOWE', 'CHUNG HING', 'CHUNG KEE', 'CHUNG ONE', 'CHUNG QUIN', 'CHUNG SUI', 'CHUNG TUNG', 'CHUNG YEN', 'CHUNG YUN', 'CINNY', 'CLARA', 'COA MOY', 'COAKLEY', 'COALOO', 'COLI', 'COLMLO', 'COLOMBO', 'COMBAR', 'COME SEE', 'COMEAL', 'COMINO', 'COMPY', 'CON BONG', 'CON SIE', 'CON TIE', 'CONDOLLY', 'CONTA', 'COOEY', 'COOK', 'COOLEY', 'COON SIN SONE', 'COONEROS', 'COORA', 'COORD COORD', 'COORY', 'COOVAL KIEE', 'COSTEPUTO', 'COURD', 'COWAL', 'COWIE', 'CREMONIA', 'CROMOW', 'CUAN QUAN', 'CUE', 'CUM CHOY', 'CUM GEE', 'CUM HOOK', 'DAD WILLIE', 'DAGI', 'DAI', 'DAISA BURE ISHIKURA', 'DANG SIC', 'DAR', 'DAVID', 'DAVIS', 'DAY', 'DAY CHONG SANG', 'DAY CHOOK', 'DAY JONG', 'DE SILVA', 'DE SILVER', 'DELECHANTOS', 'DELL', 'DEMATUS FUGIMURA', 'DIAMOND SANG', 'DICK', 'DICKSON', 'DIFEE', 'DIMOPOLOUS', 'DING SUN', 'DO YET', 'DOCTOR', 'DOLLER', 'DOMINGOS', 'DONG', 'DONG WAH LEE', 'DONNER', 'DONOW', 'DOO', 'DOO YOU', 'DOOTOR', 'DOW', 'DOW CHUNG', 'DOW HAN', 'DOW PUNG', 'DOW Senr', 'DOW TOM', 'DRASKOVITH', 'DUCH LEE', 'DUCK', 'DUCK FOO', 'DUCK SING', 'DUCK YOU', 'DUCK YOUNG', 'DUDLEY', 'DULWARVI', 'DURO', 'EDM JONG', 'EIROOS', 'EISABURO TASHIMO', 'EMRAN ALI', 'ENG FOOK', 'ENOWEIR', 'EPKANA', 'ESTEL', 'ETERO KIMINO', 'ETHERTHANGO', 'ETONG', 'ETT', 'EWED', 'FABA', 'FARUKAWA', 'FATTY MAHOMET', 'FAZIL ABDUL', 'FAZZE AEEN', 'FAZZE DEEN', 'FEE YONG', 'FEIGISUGE', 'FEN YEN', 'FENGARDIE', 'FENGUARDIE', 'FENIS', 'FERROW', 'FINNEY', 'FOKUTARO SHIMOKAWN', 'FONG', 'FONG AH LUM', 'FONG CHONG', 'FONG GEE', 'FONG HON', 'FONG KEONG', 'FONG KUE', 'FONG LEAM', 'FONG LEE', 'FONG LOCK', 'FONG LONG', 'FONG LUNG', 'FONG WAK', 'FONG WAY', 'FONG YIP', 'FOO', 'FOO CHEOO', 'FOO CHONG', 'FOO KEE', 'FOO KONG', 'FOO LEE', 'FOO YET', 'FOO YOUNG', 'FOON SING', 'FOR CHAR', 'FOR SUI', 'FOU SUE', 'FRANCISCO', 'FRASER', 'FRASER HC.', 'FREFILLY', 'FUGIMURA', 'FUMOTO', 'FUNASAKI', 'FUNG', 'FUNN', 'FURUSATA', 'GA LING', 'GALIAH', 'GAM DUCK', 'GAM HIN', 'GAM YEE', 'GAM YOUNG', 'GAMM', 'GAND FONG', 'GANG HONG', 'GANG LONG', 'GANTARA TOMOKA', 'GARIFFE', 'GARR', 'GASTON', 'GAY LEE', 'GE HOY', 'GEE', 'GEE CHONG', 'GEE HONG', 'GEE LUM', 'GEE ON', 'GEE QUONG', 'GEE WAR', 'GEE YOUNG', 'GEONG', 'GEORGE', 'GERATIS', 'GEREOGIS', 'GET HIN', 'GET PONG', 'GIMM', 'GIN SING', 'GIN WAH', 'GINDON', 'GING KIN', 'GING KIU', 'GIP HEE', 'GIZO NITTA', 'GLAM RESUL', 'GO BOW', 'GO FUN', 'GO HIM', 'GO QUAY', 'GO ROY', 'GODO', 'GOLAAM MHAND', 'GON BOW', 'GON CHU', 'GON LONG', 'GONG SANG', 'GOO CHOCK', 'GOO JUNG', 'GOOMA', 'GOON CHONG', 'GOON HEE', 'GOON LIN', 'GOONG CHONG', 'GORRIS', 'GOT JEW', 'GOW HONG', 'GOW YET', 'GOWIE', 'GOWSEEHA', 'GRAKULA', 'GRATIANO', 'GREENWOOD', 'GRUDGE', 'GUANGA', 'GUDRICK', 'GUM CHIN', 'GUM CHUCK', 'GUM LEE', 'GUM LIN', 'GUM LONG', 'GUM SING', 'GUM SUN', 'GUM TIE', 'GUM WAH', 'GUM YEE', 'GUN CHING', 'GUN LOCK', 'GUN LOEK', 'GUN TIE', 'GUN WAY', 'GUN YAN', 'GUNDAH SINGH', 'GUNE SING', 'GUY', 'GWAY', 'HA FIE', 'HACOMBE', 'HAGOSHIDA', 'HAHA', 'HAL SUE', 'HALA', 'HALEMAN', 'HALL', 'HAMADA', 'HAMAMOTA', 'HAMANO', 'HAMAT', 'HAMATNOR', 'HAMMAD', 'HAMMAT', 'HANG', 'HANG CHIN', 'HARA', 'HARK', 'HARLIE FONG', 'HARMANUS', 'HASEGAWA', 'HASHAM', 'HASHBABA', 'HASHIMOTO', 'HASSON', 'HATANA', 'HATANIK', 'HATSUGUMA MINAMI', 'HAW DOOEY', 'HAW HOP', 'HAYASHIDA', 'HAYNES', 'HE YEE', 'HEE', 'HEE YET', 'HEEBY', 'HEN QUIN', 'HEN YEK', 'HENDERSON', 'HENNICKEY', 'HERWYECE', 'HESON', 'HETARS TSUDA', 'HID', 'HIGAT', 'HIGE ODA', 'HIGUCHI', 'HILLIDEN', 'HIM', 'HINDRICK', 'HING LUM', 'HING LUM WAH', 'HING QUOCK', 'HIP CHONG', 'HIP FIE', 'HIP HING', 'HIRAKAWA', 'HIRATO', 'HIROKICHI IKEDA', 'HIRSHARA', 'HKEEN', 'HO CHING', 'HO HING', 'HO QUEN WAY', 'HO YOUNG GUN', 'HOAI', 'HOCK HING', 'HOCK HONG', 'HOCK JANG', 'HOCK LOY', 'HOCK SANG', 'HOCK SOY', 'HOCK YET', 'HODUCK', 'HOE SUE', 'HOGAN', 'HOI KEE', 'HOK YETT', 'HOLMES', 'HOMARA', 'HOME LOY', 'HON', 'HON WAH', 'HONDA', 'HONG', 'HONG CHONG', 'HONG CHOW', 'HONG DECK', 'HONG DUCK', 'HONG H. C.', 'HONG KING', 'HONG LIM', 'HONG WAH', 'HONG YET', 'HONG YOW', 'HOO PAN', 'HOO QUE', 'HOO YEUN', 'HOOK BONG', 'HOOK CHONG', 'HOOK SING', 'HOOKEY', 'HOON JANG', 'HOON RUN', 'HOONGWAR', 'HOOSMAN', 'HOP', 'HOP JANG', 'HOP LEE', 'HOP PANG', 'HOP PAW', 'HOP SEE', 'HOP SING', 'HOP WAH', 'HOP WAY', 'HOP YEK', 'HOP YONG', 'HOPP', 'HORIMY', 'HORIO', 'HORRIBOR', 'HOSIEN', 'HOSMAN', 'HOW', 'HOW CHIN', 'HOW KEE', 'HOW KUM', 'HOW WONG', 'HOWA', 'HOY', 'HOY ING', 'HOY JEE', 'HOY SUM', 'HOY TICK', 'HUCK BOW', 'HUING PIE', 'HULAY', 'HUMN HIN', 'HUNDA', 'HUNG FAH', 'HUNG WAR', 'HYASHIBARA', 'ICHIMATU NAKAMURA', 'ICK QUONG', 'IGKA', 'IGNATIS ARRIS', 'ILLARR', 'IMAKURE', 'IN FONG', 'IN FOO', 'INDIAN JACK', 'ING', 'ING CHONG', 'ING CHOY', 'INN SEE', 'ISAKICKI HOUCHI', 'ISHIP', 'ISOBA', 'ISOBE', 'ISUNYIRO KIYHONA', 'ITARO HAGIS', 'IWASA', 'IYPALO PALO', 'IZUMI', 'JACK JAPAN', 'JACKSON', 'JAMAMOTO', 'JAMBO', 'JAN BOW', 'JAN SOME', 'JANG', 'JANG BANG', 'JANG FOO', 'JANG GEW', 'JANG KAI', 'JANG LEE', 'JANG MAN', 'JANG RUN', 'JANG SEY', 'JANG THUN', 'JANG TIN', 'JANUSUKI HATADA', 'JAPARA', 'JARUM', 'JASHIZUMI', 'JASMAN', 'JAYASURIA', 'JENCAN', 'JENTARO INADO', 'JERI', 'JEUTARO FERAMOTO', 'JIM JIM', 'JIN HING SING', 'JING WAH', 'JINGO KAMASAWA', 'JINKI TANOUE', 'JINMATRU OKI', 'JINTARO KAKOSAIK', 'JIROKICHI ASAI', 'JIROR KIWASAKI', 'JIU LINN', 'JNAGORYA', 'JO JIE', 'JOCK', 'JOHANIES', 'JOHNSON', 'JON KAY', 'JONES', 'JONG', 'JONG BUN', 'JONG CHONG', 'JONG GEW', 'JONG HING', 'JONG KAI', 'JONG LUM KEE', 'JONG SAK', 'JONG SING', 'JONG TWONG', 'JONI', 'JOOYOSUS', 'JOPPA', 'JOSEPH', 'JOU', 'JOUB', 'JOW YIN', 'JOY', 'JOY LOY', 'JOYENG', 'JU FONG', 'JU FOO', 'JU HOP', 'JU JOG', 'JU LEE', 'JU WING', 'JUCHI NOMURA', 'JUE POY', 'JUITEARO KAKUSAKI', 'JUMULT', 'JUN CHOY', 'JUNG FAT', 'JUTERO FUKAI', 'KA FOOK', 'KABBAKIKEE', 'KAGETAMA', 'KAI', 'KAI KONG', 'KAJIOKA', 'KAKASUS', 'KALLAM DIBBO', 'KAMA', 'KAMADA', 'KAMAKOWA', 'KAMATZIE', 'KAN JOY', 'KAN KAY', 'KANDA', 'KANEMATU NAKAMOTO', 'KANGO OGURI', 'KANME', 'KAPA', 'KARDOLES', 'KASAI', 'KASMAN', 'KASS', 'KASSIMAN', 'KASSUP', 'KATO', 'KATSUGO HAGIMAKI', 'KATSUZO KIKAWA', 'KAVESO', 'KAWAGUSHI', 'KAY', 'KAYATI', 'KEE', 'KEE ING', 'KEE LONG', 'KEE ONE', 'KEE SEING', 'KELLAR', 'KEMSO', 'KEN DO', 'KEW JUNG', 'KEW SING', 'KIATO', 'KICHI OGURA', 'KICHIJIRO OTA', 'KICHIRO YAMAGUCHI', 'KICHIZO GOTON', 'KICK WAH', 'KIKUKIWA', 'KIKUTA SOKIBE', 'KIM JIM', 'KIM LEN', 'KIM SING', 'KIM YIN', 'KIMPE MARUOKE', 'KIMPION KAKAOKA', 'KIN KEE', 'KIN LEE', 'KIN TAI SAM', 'KING', 'KIOPEN', 'KISHURA', 'KISSEN', 'KISSENSEN', 'KISSERA WOTING', 'KITADA', 'KITAGON', 'KITANI', 'KITCHIE', 'KIYAH', 'KIYAMA', 'KODOMA', 'KOISHI', 'KOMATZ', 'KOMMAN', 'KOMURD', 'KONG', 'KONG BOW', 'KONG CHEW', 'KONG SING', 'KONG TONG', 'KONG WAH', 'KONG YIT', 'KONG YOU', 'KONG YOUNG', 'KONG YOW', 'KOOCE', 'KOONG', 'KOSAMA', 'KOTO NAWETOO', 'KOY MOTU', 'KUAHL', 'KUM HOOK', 'KUM HOOKE', 'KUM IN', 'KUM LEE', 'KUM ON', 'KUM SING', 'KUM SUNG', 'KUM WAR', 'KUM YEE', 'KUMAKICHI YAMAGUCHI', 'KUNG SUN', 'KURNARRU DE SILVA', 'KURUNARUGE DE SILVA', 'KUTSUOKA', 'KWAI CHIN', 'KWASEE', 'KWOEK YOUNG', 'KWONG CHONG', 'KWONG SANG', 'KYOJIRO KUBO', 'LAM ON', 'LAM POON', 'LAM YOU', 'LAMANKENNY', 'LAMMON', 'LAMOW', 'LANGUE', 'LATO', 'LAUNG', 'LAW FOO', 'LAW LIN', 'LAW WONG', 'LAW WOY', 'LAWSON', 'LAY', 'LAY DUCK', 'LAY SING', 'LAZARUS', 'LE CHANG', 'LE YOUNG', 'LEE', 'LEE BOW', 'LEE BUN', 'LEE BUNG', 'LEE BUTT', 'LEE CHEE', 'LEE CHEW', 'LEE CHING', 'LEE CHOW', 'LEE CHUNG', 'LEE DICK MING', 'LEE DING', 'LEE DUCK', 'LEE EIT', 'LEE FAY', 'LEE FOO', 'LEE FOY', 'LEE GAW', 'LEE GOO', 'LEE GOW', 'LEE GUM', 'LEE GUN', 'LEE HOCK', 'LEE HON', 'LEE HOP', 'LEE IN YOUNG', 'LEE ING', 'LEE JAME', 'LEE JOY', 'LEE KEE', 'LEE KIM', 'LEE KIN', 'LEE KIT', 'LEE KNONG', 'LEE KOO', 'LEE KUAY', 'LEE LAP', 'LEE LEE', 'LEE LIE', 'LEE LOOK', 'LEE LYE', 'LEE MEE', 'LEE MONG', 'LEE MOON', 'LEE ON', 'LEE PAN', 'LEE PING', 'LEE POO', 'LEE POY', 'LEE QUAY', 'LEE QUIN', 'LEE SANG', 'LEE SEE', 'LEE SEE TIE', 'LEE SHEU', 'LEE SHEW', 'LEE SIN', 'LEE SING', 'LEE SOM', 'LEE SON', 'LEE SUE', 'LEE SUN', 'LEE SUNG', 'LEE UNGUM', 'LEE WAR', 'LEE WAY', 'LEE WIA', 'LEE WING', 'LEE YEE', 'LEE YIN', 'LEE YOU', 'LEE YOUGH', 'LEE YOUNG', 'LEE YOW', 'LEE YUM', 'LEELAP', 'LEHARA', 'LENCONCIA', 'LEO', 'LEO MAU', 'LEONDARAKIS', 'LEONG', 'LEONG CHIP', 'LEONG DYE', 'LEONG GAIM', 'LEONG GEE', 'LEONG GON', 'LEONG HOY', 'LEONG JEN', 'LEONG JIEM', 'LEONG SING HC.', 'LEONG SINGE', 'LEONGSO', 'LEU GANG', 'LEUNGMUN', 'LEVENA', 'LEW HOY', 'LEW TOO', 'LEWIE', 'LEWIS', 'LI HUNG', 'LIEVALSUM', 'LIM BAH', 'LIM GIP', 'LIM KEE', 'LIM KIN', 'LIM YUN', 'LIN FONG', 'LIN GET', 'LIN HOP', 'LIN SEY', 'LIN TIE', 'LIN WON', 'LIN YAI FOO', 'LIN-SU', 'LING GEE', 'LING KEW', 'LIP SEE', 'LIU TUCK', 'LIY', 'LLOYD', 'LO CHEW', 'LO HOON', 'LO LIN', 'LO QUAY', 'LO WOO', 'LOCOSSIE', 'LOE TERARE', 'LOGGIE', 'LOGOMIER', 'LOGOTHETIS', 'LON SUE', 'LONE', 'LONG', 'LONG CHONG', 'LONG CHUNG', 'LONG FOOK', 'LONG GONG', 'LONG HONG', 'LONG KWONG SANG', 'LONG LEN', 'LONG ON', 'LONG TYE', 'LONG WAY', 'LONG YEE', 'LONGFELLOW', 'LOO FAT', 'LOO NIN', 'LOO WING', 'LOOK', 'LOOK HING', 'LOOK NGIN', 'LOOK PING', 'LOOK SOO', 'LOOK WING', 'LOOKHOOP', 'LOONG SING', 'LOU HONG', 'LOU SUN', 'LOU TIN IT', 'LOUE', 'LOUEY', 'LOUM MOO', 'LOVLY', 'LOW', 'LOW BAN', 'LOW BUCK', 'LOW CHARE', 'LOW CHEW', 'LOW CHING', 'LOW CHONG', 'LOW CHOY', 'LOW CHUNG', 'LOW CHUT', 'LOW CUM', 'LOW DING', 'LOW FONG', 'LOW FOO', 'LOW GET', 'LOW GUM', 'LOW GUY', 'LOW HEE', 'LOW HOOK', 'LOW HOY', 'LOW JON HOOK', 'LOW KING', 'LOW MOW', 'LOW PING CHONG', 'LOW PUN', 'LOW QUAY', 'LOW SANG', 'LOW SHOONG', 'LOW SING', 'LOW TEOONG', 'LOW WAN', 'LOW WING', 'LOW YEE', 'LOW YIN', 'LOWE FIRE', 'LOWTALL', 'LOY QUONG', 'LOY SOW', 'LU SING', 'LUCE', 'LUE CHUT', 'LUIE MOON', 'LUM', 'LUM BANGLIU', 'LUM CHEW', 'LUM CHOW', 'LUM CHOY', 'LUM DONG', 'LUM FONG', 'LUM FUN', 'LUM GARP', 'LUM GEW', 'LUM GOON CHONG', 'LUM GUN', 'LUM HING', 'LUM HOP', 'LUM JOY', 'LUM KEE', 'LUM KIN', 'LUM KUM', 'LUM LEE', 'LUM LIM', 'LUM LOW', 'LUM LUP', 'LUM MEW', 'LUM MUG', 'LUM NI', 'LUM SEE', 'LUM SHONG', 'LUM SIN', 'LUM SING', 'LUM SUM', 'LUM TART', 'LUM WAN', 'LUM WING', 'LUM YAN', 'LUM YET', 'LUM YICK', 'LUM YOU', 'LUNG BUN', 'LUY LUP', 'LYTORIA', 'MA HOM', 'MABLAM', 'MACK CHEW', 'MACK DET', 'MACK YOCK', 'MACREE', 'MADAM', 'MADDER', 'MADRAS', 'MAGE', 'MAGIE', 'MAGO SAMURA', 'MAGOSABURA NATOMI', 'MAH DAY', 'MAH FONG', 'MAH GON', 'MAHOMET ALI', 'MAHOMET HAFFIS', 'MAI', 'MAI MI', 'MAINARDT', 'MAJOR', 'MAKALIEO API', 'MAKEELA', 'MAKINO', 'MALA KAI', 'MALARO', 'MALAY', 'MALDUIE', 'MALICOOLA', 'MALICOOLE', 'MALIKOLO', 'MALLAMER', 'MALLETNOW', 'MALOCKER', 'MALOUF', 'MAMDEEN', 'MAMOOASSIE', 'MAN CHAN', 'MAN GETT', 'MAN JAME', 'MAN MOON', 'MAN WAH', 'MANAJACKA', 'MANAKA', 'MANAWAKAKE', 'MANDA', 'MANEBORO', 'MANFURUNIS', 'MANGOI', 'MANNAWAH', 'MANNESEE', 'MANOVER', 'MANSOMBA', 'MAR CHONG HING', 'MAR FAN', 'MAR JEW', 'MAR JOY', 'MAR KEE', 'MAR KONG', 'MAR LUNG', 'MAR QUAY', 'MAR SUN', 'MAR YIN', 'MARANIO', 'MARATTA', 'MARAWATTA', 'MARAYATTA', 'MARGEE', 'MARI', 'MARIGA', 'MARKAGEE', 'MARLEE', 'MARLOW', 'MARRADEM', 'MARRATTA', 'MARTEE', 'MARTEN', 'MASAICHI IZUMI', 'MASATA AGATA', 'MASMOTO', 'MASSA', 'MASSEY', 'MASUMOTO', 'MATA', 'MATEURVA', 'MATHA', 'MATSEWOREY', 'MATSUMI UYEMITSU', 'MATSUNA', 'MATSUSKIMO', 'MATTASAN', 'MATUISCHI OKU', 'MAULA', 'MAW LEE GAW', 'MAY', 'MAYADA', 'MAYAO', 'MAYDO', 'ME YOW', 'MEAGSUMOTO', 'MEDLAP', 'MEE HOO', 'MEE HUOON', 'MEE LAW', 'MEE LING', 'MEE SI', 'MELLICK', 'MEN HONG', 'MENNOW', 'MENO KICHI WEYIDA', 'MEON', 'MEREDITH', 'MERRYFOR', 'MERUBOOBOO', 'METABE FURUKAWA', 'METHANITIS', 'MEW CHUN', 'MEW YECK', 'MICHAEL', 'MILAND', 'MILLER', 'MIN CHIN', 'MING', 'MINGO', 'MINON', 'MITAKARA', 'MIYABE', 'MIYAKIEKI FURUTO', 'MIZZEN', 'MO HING', 'MOCK WAY', 'MOFFAT', 'MOHOMED DEEN', 'MOKOMUN', 'MOLAY', 'MOLIBACK', 'MON FAY', 'MON GUN', 'MON HIN SANG', 'MON HING', 'MON ON', 'MON QUAY', 'MONDABIE', 'MONDAY', 'MONGA', 'MONN MOSS', 'MONOLI', 'MONT CHOY', 'MOOK GAW', 'MOOLEETHA', 'MOON QUAN', 'MOON SHEE', 'MOONEY', 'MOOR TEE', 'MOORE', 'MORASANY', 'MORATTA', 'MOREY', 'MORI', 'MORITA', 'MOSES', 'MOTA', 'MOTLAP', 'MOW CHEW', 'MOW HOU ?', 'MOW HOW ?', 'MOW KWAN', 'MOW SING', 'MOW TING', 'MOW YEE', 'MUD FAT', 'MUIRA', 'MULLBERRY', 'MULLISUM', 'MUN HON', 'MUNDY YABON', 'MUNSA SINGH', 'MURAKIMA', 'MURGASSON', 'MURIKAWA', 'MUSTARD ?', 'MUTTING', 'MUTTON', 'MY DEAR VEA', 'MYLUNG', 'MYVO', 'McKENZIE', 'NA HOY', 'NABBY BUX', 'NAHAMURA', 'NAKADA', 'NAKAGOWA', 'NAKAGUTCHA', 'NAKAHAMA', 'NAKANISHI', 'NAKASHAMIA GAZO', 'NAKASHIMA', 'NAKASONE', 'NALAY', 'NAMI', 'NAMURA', 'NANA', 'NANA SINGH', 'NAPIO', 'NARBUNG', 'NARKEEK', 'NARLYA', 'NARRA', 'NARROWA', 'NARSMID', 'NASSER', 'NATSU HARA', 'NAVES', 'NAVISPES', 'NE GOUY', 'NEGO', 'NEGOWAY', 'NELLOP', 'NELLSSEN', 'NEWANT', 'NICSUS', 'NIEHOLAS MESSUES', 'NING', 'NISHI', 'NISHIMURA', 'NISHITI', 'NISTINIOTO', 'NITARA', 'NOAH SABBO', 'NOAM', 'NOBU TANAKA', 'NOELAND', 'NOGANAWA', 'NOGAR', 'NOKO', 'NOMPUA', 'NONGI', 'NOSAWMA', 'NOTAKAR', 'NOURI', 'NOWATER', 'NOWMONDY', 'NUMBACAN', 'NUMM', 'O PHEE', 'OABA', 'OBA', 'OBAYUSHI', 'ODINAMARAUDA', 'OGATA TAKESHI', 'OGISO', 'OGURA', 'OGURA SINHITI', 'OH CHAN', 'OHANEER', 'OHTELLWO', 'OISHI', 'OKADA', 'OKAMI', 'OKOOMORA', 'OKUDA', 'OKURA', 'OLEHOWE', 'ON', 'ON HING', 'ON SING', 'ON SIY', 'ON YAN', 'ON YONG', 'ONA', 'ONAH', 'ONDOO', 'ONE', 'ONEMIRE', 'ONN', 'ONO', 'ONTONG', 'OOBA', 'OOTAY', 'ORELLA', 'ORMERIN', 'OSAKI', 'OTOKAWA', 'OTOKIHI JINMAI', 'OTTO MATURA', 'OUTO', 'OVEESA', 'OVETT', 'OYAMEA', 'PACK GEE', 'PALMER', 'PAN HEE', 'PAN LIN', 'PAN SAM', 'PANKEE', 'PATER', 'PATHER', 'PAULINA', 'PAW WAH', 'PEDERMAN', 'PENOTAH', 'PENTECOST', 'PETO BELOOCH', 'PICTRO', 'PILIS', 'PING', 'PING YOUNG', 'PMOE', 'POI KEE', 'POLAR', 'POLLWALY', 'PONG', 'PONG GEE', 'PONG SUNG', 'POOLAR', 'POON', 'POON LANGM', 'POPADOPOLOS', 'POWELL', 'POY', 'PRACA', 'PRATT', 'PREIRA', 'PRINCE BUTLER', 'QUALAMIBER', 'QUAN', 'QUAY', 'QUAY CHOW', 'QUAY FONG', 'QUERRO', 'QUETTA', 'QUIN', 'QUINTER', 'QUN HIN', 'QUO HING', 'QUONG AH TONG', 'QUONG CHONG', 'QUONG DONG', 'QUONG PIE', 'QUONG TEY', 'QUONG WING', 'QUTARO NISHIMURA', 'RABEO', 'RABIN', 'RABING', 'RAMBLINE', 'RANAWERA', 'RANNAN', 'RAROO', 'RAUHECABULL', 'RAVA', 'RAVENO', 'RAYTIM', 'REAM KHAN', 'REAM KHAN FAZZE AEEN', 'REAM KHAN FAZZE DEEN', 'RENOW', 'ROSSA', 'ROSSO', 'ROW WONG', 'ROWDY', 'RUB CHUN', 'RUBY', 'RUDDY', 'RURU', 'SABBO', 'SABURA HARUNO', 'SABUROMAROU', 'SACHOULIS', 'SAFFEY', 'SAGA', 'SAHARA', 'SAIZU MIYOSHI', 'SAKA', 'SAKAE', 'SAKAMOTA', 'SAKATA', 'SAKELLAROPOULOUS', 'SAKU MORI', 'SAKUMA', 'SAKUTA SHIBATA', 'SALAM', 'SAM', 'SAM KEE', 'SAM LEE', 'SAM LEON', 'SAM MURRAY', 'SAM WAH', 'SAMACK', 'SAMON', 'SAMUELS', 'SAN LEE', 'SAN LIN', 'SANDY', 'SANG', 'SANGI SAKATI', 'SANGYOU', 'SANNON', 'SANTA', 'SANTARO HAMA', 'SANTO', 'SARAVEE', 'SARBAU', 'SARDIE', 'SAREMON', 'SARIM', 'SARJUN', 'SARMADI', 'SARRAHAMOO', 'SARTICHER', 'SASAKI', 'SAY HING', 'SAY KONG', 'SAY LIN', 'SCHLICE', 'SCHNATCHIE', 'SCHWELAN', 'SCHY', 'SCKUTARO NODA', 'SEADORIOUS', 'SEE', 'SEE FOOK', 'SEE GA', 'SEE HING', 'SEE HONG', 'SEE HOY', 'SEE HUNG', 'SEE KONG', 'SEE LEE', 'SEE LOOP', 'SEE LOW', 'SEE M HOOK', 'SEE MAN', 'SEE MOON', 'SEE MOW', 'SEE OONG', 'SEE QUIN', 'SEE SO', 'SEE WAH', 'SEE YONG', 'SEE YOU', 'SEEDEN', 'SEEK DOMEN', 'SEEKIS', 'SEEMON', 'SEEWON', 'SEGEMEMTO', 'SEIGH', 'SELIM', 'SELVER', 'SENJIRO SHIMADA', 'SENO DEGORO', 'SERIGAH', 'SETO', 'SEVEN', 'SHAMISTOKLES COSTEPUTO ?', 'SHAR', 'SHAR MAHOMED', 'SHARA', 'SHARAN', 'SHARK', 'SHEDIN', 'SHI EMO', 'SHIMIZU', 'SHIMMAMURA', 'SHIMO', 'SHINIZU', 'SHINPACHI INAUE', 'SHIRAHI', 'SHIRAKI', 'SHITASAKO', 'SHIZUMURA', 'SHIZUNO HONDA', 'SHOMAR', 'SHUKISCHI YAMADA', 'SHUN TUNG', 'SHUNG TART', 'SICENDER', 'SIDDON', 'SIDORIS APPOO', 'SIE CHOW', 'SILOVA', 'SILOVO', 'SILVA', 'SILVA MARTIN', 'SIM', 'SIMEN', 'SIMS', 'SIN CHIN', 'SIN GUTT', 'SIN HOY', 'SIN MAN HANG', 'SIN ON LEE', 'SIN YOU', 'SINDEN', 'SINEM', 'SING', 'SING CHONG', 'SING HOW', 'SING LIN', 'SING LOY', 'SING ON', 'SING QUAY', 'SING TOY', 'SING WAY', 'SING WING', 'SING WING SUE YEK', 'SING YOU', 'SINGA APPOO', 'SINGE', 'SIPPIE', 'SIREN', 'SISORY', 'SIT KHAN', 'SIU YOU', 'SIY HOCK', 'SMITH', 'SO CHIN', 'SOLOMN', 'SOLOMON', 'SON GUN', 'SONEN', 'SONG HONG', 'SONGHE HOP YEK', 'SOO SOO', 'SOORAW LORSE', 'SOSEEHAH', 'SOURAN', 'SOUTAVERE', 'SOW HOO', 'SOW KEE', 'SOW KIN', 'SOW KONG', 'SPATHIS', 'STAMATIS', 'STEPHENS', 'STONG', 'SUBA', 'SUC JUNG', 'SUCK YOU', 'SUCSOKOO', 'SUE', 'SUE BON', 'SUE CHUCK', 'SUE GUM', 'SUE GUY', 'SUE LOOK', 'SUE LYE', 'SUE SEE', 'SUE SING', 'SUE SUNG', 'SUE TIN', 'SUE TYE', 'SUE YEP', 'SUE YEUN HOP', 'SUE YUM', 'SUEKIEHI SHINTO', 'SUI CHOY', 'SUI WAH', 'SUIKIHI SOGAMA', 'SUINAMOOTY', 'SUM LUN', 'SUM MAN LONG', 'SUME', 'SUMIZO OKAMATU', 'SUMOR', 'SUN', 'SUN CHONG LOONG', 'SUN CHONG WAH', 'SUN HIN', 'SUN HOP', 'SUN JONG', 'SUN KEE', 'SUN LUNG', 'SUN MEE', 'SUN NAM', 'SUN SAM SING', 'SUNBUX', 'SUNNIE KHAN', 'SUNTOP', 'SURAT', 'SURRA HASSAN', 'SUT HOI KEE', 'SUT KEE', 'SUTEMATSU TANAKA', 'SWAGGY', 'SYDNEY YATTA', 'SYDNON', 'SYMON', 'TABBY', 'TABERIS HEMUI', 'TABHE', 'TABOOSY', 'TAITERS', 'TAK PUI', 'TAKAGAKI', 'TAKAHASHI', 'TAKAKI', 'TAKAMOTO', 'TAKATA', 'TAKCHI OZAWA', 'TAKEGIRO SHIMADA', 'TAKEHARA', 'TAKIDA', 'TAKOO', 'TALEWIE', 'TALLIS', 'TAM HC.', 'TAMARI', 'TAMBO', 'TAMIKISHI TAKATA', 'TANAKA', 'TANGAWA', 'TANNA', 'TANNER', 'TAPOONA', 'TARA', 'TARAKICHI KUMISKO', 'TARAMOOR', 'TARANDO', 'TARKA', 'TARLOCH', 'TARLONGA', 'TARMIKIEHI', 'TAROICHI NISHI', 'TAROMAI', 'TARRALOO', 'TARRIALLA', 'TARRIELLEMA', 'TARRYANGO', 'TARRYGWIDYOR', 'TASMAL', 'TASS', 'TASUHARA', 'TATERS', 'TATOW', 'TATSUJIRO NAKATA', 'TATSUMI', 'TAVAGIM', 'TAVELLY', 'TAVITEE', 'TAYLOR', 'TEACKER', 'TEAMIKICHI', 'TEHERO', 'TEMANI', 'TEMBOAN', 'TENNOW', 'TESSIP', 'TEUGUANDA', 'TEUKATA', 'THOR', 'THUN', 'TIA', 'TIBBY', 'TIE', 'TIGER', 'TILBY', 'TIM', 'TIMBARNOW', 'TIN', 'TIN SIN', 'TIY', 'TOATON', 'TOCK', 'TOEWAN', 'TOKI', 'TOKISUKI', 'TOKUSO', 'TOLKI', 'TOLOA', 'TOMARROW', 'TOMATTO', 'TOMIKIE', 'TON', 'TONG', 'TONG SAM', 'TONGA', 'TONGHA', 'TONKABO', 'TONOR', 'TOO-TOO-E', 'TOOAVELEA', 'TOOMY', 'TOONG', 'TOOSHOO', 'TORAHKASEA', 'TOWLEY', 'TOWN', 'TOY', 'TOY LOY', 'TOYAMA', 'TOYER', 'TOYOTARA', 'TRUQUANNIE', 'TSUBOSHIMI', 'TUDER', 'TUNEHERO', 'TUNEKI', 'TUNG', 'TUNG YEEN', 'TURRY', 'TURUNJA', 'TY', 'UATTO', 'UBI', 'UK', 'UKICHI', 'UMATARA', 'UMIKICHI', 'UNOSUKE', 'USIMURKA', 'UTARA', 'VEELEE', 'VEETEE', 'VELEE', 'VELLI', 'VENDELO', 'VERA', 'VERINAL', 'VETON', 'VIEN', 'VURNATT', 'WAEN', 'WAH', 'WAH CHANG', 'WAH COME', 'WAI', 'WAIT', 'WAKAZONO', 'WAKIMATA', 'WALLAH', 'WALTERS', 'WAN', 'WANG', 'WAR', 'WARAMARAB', 'WARCON', 'WARKILL', 'WARR', 'WASHA', 'WASUAK', 'WATANABE', 'WATARI', 'WATHAKEN', 'WATSON', 'WATTOO', 'WAY', 'WAY HUNG', 'WAYAM', 'WEDEN', 'WEE', 'WEEIPO', 'WEIROW', 'WEKAIA', 'WELLS', 'WEN', 'WETAL', 'WEYNO', 'WHATAWORT', 'WHO', 'WHO HANG', 'WILL', 'WILLIAMS', 'WILLOWS', 'WILLS', 'WILLTOWLEE', 'WINDIA', 'WING', 'WING KEE', 'WISHER', 'WOM', 'WON', 'WONAM', 'WONG', 'WONG FOO', 'WONG RIGHT', 'WONG SHUN', 'WONG YEP', 'WOO', 'WOOD', 'WOODHAM', 'WOODS', 'WOOLWOOL', 'WOREMP', 'WORROWAY', 'WOSARE', 'WRIM', 'WYAH', 'WYEHARA', 'WYMERIA', 'YABUTA', 'YAGUMA', 'YAICKIRO', 'YALU', 'YAM', 'YAMAGUCHI', 'YAMAHITA', 'YAMANAKA', 'YAMATO', 'YAMOMOTO', 'YAN', 'YAN GET', 'YAN LOW', 'YANDAR', 'YANG', 'YANK YANK', 'YARAFEE', 'YARHEHEELO', 'YARLOW', 'YASSARRIE', 'YASSO', 'YASUTARO', 'YATOOPOOKOO', 'YAW SING', 'YE HOP', 'YEE CHONG', 'YEE DAY', 'YEE FONG', 'YEE FUNG', 'YEE HONG', 'YEE HOP', 'YEE ICK', 'YEE JON', 'YEE JOY', 'YEE LAN', 'YEE MEM', 'YEE PAR', 'YEE PING', 'YEE SING', 'YEE SOW', 'YEE TOCK', 'YEE WAH', 'YEE WAN', 'YEE YOW', 'YEH OP', 'YEN BOW', 'YEN DUCK', 'YEN FOO', 'YEN KAY', 'YEN KEE', 'YEN OAN', 'YEN QUAY', 'YEN QUIN', 'YEN SEN', 'YEN WAH', 'YEN YEE', 'YET', 'YET CHEW', 'YET FOY', 'YET LEE', 'YET MUROA', 'YET MWOA', 'YET WAH', 'YETARO OYE', 'YETO', 'YEU HOP', 'YHOWGOW', 'YIN FOO', 'YIN GUY', 'YOCK CHIN', 'YOGON SHIN', 'YOGOS NAKAYAMA', 'YOKE MOWE', 'YOKICHI ENDO', 'YOKOTA', 'YOKOYAMA', 'YOMAMOTA', 'YONG CHIN', 'YONG CHOY', 'YONG FOOK', 'YONG MUN', 'YONGE TIE', 'YOOK KEE', 'YORK SUN', 'YOSHIDA', 'YOSHORO TINIAKA', 'YOU', 'YOU FEE', 'YOU HOY', 'YOU LEE', 'YOUEMITSU', 'YOUEN GON', 'YOUETARO IWAMOTO', 'YOUNG', 'YOUNG CHOY', 'YOUNG FATT', 'YOUNG GEE', 'YOUNG HOOK', 'YOUNG KEEN', 'YOUNG KOO', 'YOUNG LEE', 'YOUNG LIN', 'YOUNG QUNG', 'YOUNG SAY', 'YOUNG SEE', 'YOUNG SING', 'YOUNG TONG', 'YOUNG WAY', 'YOUNG WING', 'YOUSE', 'YOW', 'YOW CHEW', 'YOW HING', 'YOW LEE', 'YOW YEH', 'YOW YEH Jnr', 'YOW YEH Snr', 'YUCK WAH', 'YUCKMAN', 'YUEN', 'YUM', 'YUN DOW', 'YUN WAH', 'YUNG KOO', 'ZAMBE', 'ZANGLAS', 'ZANZEBAR', 'ZEMERIS', 'ZIMMIE', 'n/a']</t>
         </is>
@@ -574,18 +591,26 @@
       <c r="P3" t="n">
         <v>3</v>
       </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>na</t>
-        </is>
-      </c>
-      <c r="R3" t="n">
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="T3" t="n">
         <v>12674</v>
       </c>
-      <c r="S3" t="n">
+      <c r="U3" t="n">
         <v>416</v>
       </c>
-      <c r="T3" t="inlineStr">
+      <c r="V3" t="inlineStr">
         <is>
           <t>['1977', '2', 'A', 'A R', 'Abdul', 'Abraham', 'Abram Yarad', 'Ada', 'Agnes', 'Ah Moy', 'Aheeba', 'Albert', 'Albert Mark', 'Alec', 'Alex', 'Alexander', 'Alexis', 'Alfred', 'Alice', 'Alice Florence', 'Alice Maude Victoria', 'Alick', 'Alikke', 'Alvina', 'Amy', 'Andrew', 'Andy', 'Angelo', 'Annie', 'Anst', 'Anthony', 'Antoni', 'Antonia', 'Arthur', 'Arthur Shik', 'Assid', 'Azze', 'B', 'Baba', 'Barbara', 'Ben', 'Bene', 'Bernie', 'Bertha', 'Bertie', 'Bessie', 'Bettssey', 'Bewah', 'Billy', 'Bob', 'Bobby', 'Bow', 'Bun', 'C', 'Caroline', 'Catherine', 'Catherine Emily Rosena', 'Cecelia', 'Cecil', 'Chan', 'Charles', 'Charley', 'Charley Henry', 'Charli', 'Charlie', 'Charlie Allen', 'Charlie Luke', 'Charlie Raymond', 'Charlie Sam', 'Charlie Simon', 'Charlotte', 'Chas Luke', 'Checkar', 'Chin', 'Ching', 'Chong', 'Chow', 'Choy', 'Christina Olivia', 'Chut', 'Cissy', 'Claude', 'Claude H', 'Con', 'Constantine', 'Crea...y', 'D', 'Dan', 'Dang', 'Daniel', 'David', 'Davy', 'Day', 'Demetrus', 'Dennis', 'Denny', 'Dick', 'Die', 'Don', 'Dong', 'Donnie', 'Doris', 'Dorothy', 'E', 'E Jane', 'Eat', 'Eddie', 'Edith', 'Edward', 'Eileen', 'Eli', 'Elias', 'Eliza', 'Elizabeth', 'Ellen', 'Ellen Ann', 'Ellien', 'Elsie', 'Emily', 'Emma', 'Ernest', 'Eva', 'Evie', 'F', 'Fanny', 'Farreen', 'Fat', 'Femelia', 'Fong', 'Foon', 'Francis', 'Frank', 'Frank Francis', 'Frank J Sam', 'Fred', 'G', 'Geava', 'Gee', 'George', 'George Daker', 'George Gong', 'George Moses', 'Georgi', 'Georgie', 'Gertrude', 'Ghee', 'Gib', 'Gilbert', 'Gip', 'Good', 'Gook', 'Goon', 'Gow', 'Grace', 'Gun', 'H', 'H C', 'Hanasha', 'Harold', 'Harry', 'Harry Andrew', 'Harry Sam', 'Hendrich', 'Henry', 'Herbert', 'Hing', 'Ho', 'Hock', 'Hop', 'Hore', 'How', 'Hugh', 'Hunter', 'I', 'Ida', 'Inn', 'Iris', 'Isaac', 'Issaka', 'Ivy', 'J', 'Jack', 'Jack Sam', 'Jacob', 'James', 'James Douglas', 'James Sam', 'James Y', 'Jean', 'Jeanie', 'Jemima', 'Jemma', 'Jemmy', 'Jennie', 'Jenny', 'Jessie', 'Jessy', 'Jim', 'Jimmie', 'Jimmy', 'Jing', 'Jinny', 'Joe', 'John', 'Johney', 'Johnie', 'Johnnie', 'Johnny', 'Jonas', 'Jonny', 'Joseph', 'Joseph David', 'Joseph Lucas', 'Jot', 'Joung', 'Joy', 'Julia', 'K', 'K C', 'K.', 'Karma', 'Kathleen', 'Katie', 'Kee', 'Kew', 'L', 'Lap', 'Larrie', 'Larry', 'Lee', 'Leong', 'Lester Henry', 'Lillian', 'Lin', 'Ling', 'Lizzie', 'Long', 'Look', 'Louie', 'Louie Eugene', 'Louis', 'Loy', 'Lucy', 'Luke', 'Lum', 'Lyla', 'M', 'M.', 'Madeline', 'Maggie', 'Maikawa', 'Margaret', 'Martha', 'Mary', 'Mary Agnes', 'Masuda', 'Matthew', 'Matumure', 'Maud', 'Maudie', 'May', 'Mealkie', 'Michael', 'Mick', 'Mijizaki', 'Minnie', 'Mitchel', 'Mitunaga', 'Mo Hing', 'Mow', 'Mrs', 'Muriel', 'Myria', 'N', 'Nagla', 'Nasta', 'Ned', 'Nellie', 'Nicholas', 'Noel', 'Norah', 'Norman', 'O', 'Okayama', 'Olive', 'On', 'Osaki', 'Ow', 'P', 'Patema', 'Paul', 'Percy', 'Peter', 'Phillip', 'Phylis', 'Phylliss', 'Ping', 'Pong', 'Quay', 'Queenie', 'Quin', 'Quoy', 'R', 'R G', 'Rachel', 'Robert', 'Robert Bob', 'Rose', 'Rosena', 'Rosie', 'Ruby', 'Rupert', 'S', 'S Wm', 'Sade', 'Sam', 'Sam Charlie', 'Sam Willie', 'Sammy', 'Samuel', 'Samuel Charles', 'Sando', 'Sandy', 'Sang', 'Sarah', 'Say Ning', 'See', 'Selam', 'Sellem', 'Selma', 'Seper', 'Seundra', 'Shanistokles', 'Simon', 'Sin', 'Sing', 'Sissie', 'Sitee', 'Son', 'Soo', 'Sop', 'Stanley', 'Stephen', 'Sue', 'Sueie', 'Sun', 'Sung', 'Susan', 'Susie', 'Susy', 'Suzie', 'Sydney', 'T', 'T A', 'Takehara', 'Tamami', 'Tammy', 'Tango', 'Tanny', 'Theadore', 'Theorodo', 'Thom', 'Thomas', 'Thos Yeek', 'Tiem', 'Tim', 'Tin', 'Toby', 'Tom', 'Tomie', 'Tommy', 'Tommy Norman', 'Tomy', 'Ton', 'Topsy', 'Tow', 'Tsueng', 'Turuda', 'U', 'U.', 'Uyemura', 'V', 'Vera', 'Violet', 'Vivian', 'W', 'Wada', 'Wagh', 'Wah', 'Walter', 'Washa', 'Way', 'Wedada', 'Westeria', 'William', 'William Daniel', 'William John', 'Willie', 'Willie Sam', 'Willy', 'Wylie', 'Y', 'Yarad', 'Yee', 'Ying You', 'Yip', 'Yock', 'Yong', 'Yoo Sun', 'Youm', 'Young', 'Yow', 'Yung', 'Yup', 'n/a', 'na']</t>
         </is>
@@ -644,18 +669,26 @@
       <c r="P4" t="n">
         <v>0</v>
       </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="R4" t="n">
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>China</t>
+        </is>
+      </c>
+      <c r="T4" t="n">
         <v>30455</v>
       </c>
-      <c r="S4" t="n">
+      <c r="U4" t="n">
         <v>244</v>
       </c>
-      <c r="T4" t="inlineStr">
+      <c r="V4" t="inlineStr">
         <is>
           <t>['117', '188', '345', '38', '9', 'Adelaide', 'Aden', 'Afghanistan', 'Africa', 'Albert River', 'Althans Greece', 'Amakasa Japan', 'Ambrayan', 'Ambrim', 'Ambrym', 'Ambrym Island', 'Ambyrim', 'America', 'Amoy China', 'Aoba', 'Aoba South Sea Islands', 'Api', 'Arabia', 'Aramac Queensland', 'Aramango Island', 'Armando Island', 'Asia', 'Assyria', 'Athens', 'Atherton', 'Ave Isd', 'Ave Island', 'Ayr', 'Ayr Queensland', 'Batavia', 'Bombay', 'Bombay India', 'Bowen', 'Bowen  Qland', 'Bowen  Queensland', 'Bowen Queensland', 'Brisbane', 'Brisbane Queensland', 'British Portion of Syria', 'Bucca Bucca Island', 'Bundaberg Queensland', 'Byroot Seerea', 'Calcutta', 'California', 'California America', 'Callatmatto', 'Calliope Queensland', 'Can Tong China', 'Canton', 'Canton  China', 'Canton China', 'Cape de Verde Islands', 'Ceylon', 'Ceylon India', 'Chan Hang China', 'Charaway', 'Charleville Queensland', 'China', 'Chunghi China', 'Cirago', 'Colombo', 'Constantinople', 'Constantinople Syrian', 'Cooktown', 'Cooktown Queensland', 'Coorooman', 'Coorooman Queensland', 'Corfue', 'Croydon', 'Cumberland', 'Cunnamulla', 'Dalby Queensland', 'Damaskis', 'Don Goon China', 'East India', 'Ebey Island', 'Egypt', 'Emu Park', 'Emu Park Queensland', 'Eppie Island', 'Euthella', 'Fiji Islands', 'Frazer Island', 'Fukuoka Japan', 'Futoona Island', 'Gala', 'Georgetown', 'Girgi Greece', 'Girigi Greece', 'Gladstone', 'Goondi Queensland', 'Gowell', 'Greece', 'Gungong China', 'Halifax Queensland', 'Hang Shan China', 'Hebrides', 'Herbert River  Queensland', 'Hippi Island', 'Hong Kong', 'Hong Kong China', 'Hong San China', 'Hong Sang China', 'Hong Sing China', 'India', 'Ingham', 'Ingham  Queensland', 'Ingham Queensland', 'Ingham Queesnland', 'Jamaica', 'Japan', 'Java', 'Kades Syria', 'Kanaka', 'Kinishu', 'Kobe Japan', 'Kwang Tung China', 'Lacane Island', 'Lacarie Island', 'Lacona Island', 'Laf Kas Greece', 'Lahore  India', 'Law Island', 'Levan', 'Levo New Caledona', 'Lismore New South Wales', 'Mackay  Queensland', 'Mackay Queensland', 'Madras', 'Malay', 'Malicola', 'Malicoola', 'Mallacooller Island', 'Manilla', 'Marata Island', 'Maratta', 'Marcow Canton China', 'Maritius', 'Marlow', 'Mauritius', 'Merider Island', 'Mia Island', 'Monortine Turkey', 'Montenegro', 'Moratta I', 'Mornish Queensland', 'Mortlap Island', 'Mount Labenon', 'Mount Lebnon Flaly', 'Mullacoola', 'Murray Island', 'Myreken', 'Nagasaki Japan', 'Nan Shan China', 'Nanbin Queensland', 'New British Island', 'New Caladonia', 'New Caledonia Island', 'New Hebrides', 'New Isd', 'New Island', 'New Orleans America', 'New South Wales', 'New Zealand', 'Oba', 'Oba Island', 'Orange New South Wales', 'Palestine', 'Palmer Island', 'Pekin China', 'Pentecost Island', 'Penticost', 'Peruo', 'Peshawar', 'Phillipine Island', 'Phillipine Islands', 'Pikedale Warwick', 'Port Darwin', 'Port Darwin South Australia', 'Port Seria Syria', 'Portugal', 'Proserpine  Queensland', 'Punjab India', 'Punjaub India', 'Punquab India', 'Qld', 'Queensland', 'Rockhampton', 'Rockhampton Queensland', 'Roma', 'Rome Italy', 'Samoa', 'Samoa Island', 'Samos Turkey', 'Sandhills', 'Sandhills Queensland', 'Sandwich Island', 'Sandwich Islands', 'Santo Id', 'Santo Island', 'Saples Turkey', 'Satsuma Japan', 'Shan High China', 'Singapore', 'Singapore Malay', 'Sinon China', 'Solomon', 'Solomon Island', 'Solomon Islands', 'South America', 'South Sea Islands', 'St George', 'Stanthorpe Queensland', 'Syria', 'Tanna Island', 'Tanna Islands', 'Tenterfield New South Wales', 'Texas Queensland', 'Thessily Greece', 'Thursday Island', 'Tinga New South Wales', 'Tivoli Ipswich', 'Tokio', 'Tokio Japan', 'Tokolo Island', 'Tonor Island', 'Toowoomba', 'Toowoomba Queensland', 'Townsville', 'Tripoli Asyria', 'Turkey', 'Veritic Greece', 'Wakayama', 'Wakaymapen Yanabe Japan', 'Warwick', 'Warwick Queensland', 'West Indies', 'Yong Hong China', 'n/a']</t>
         </is>
@@ -714,18 +747,26 @@
       <c r="P5" t="n">
         <v>4</v>
       </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="R5" t="n">
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="T5" t="n">
         <v>7099</v>
       </c>
-      <c r="S5" t="n">
+      <c r="U5" t="n">
         <v>4</v>
       </c>
-      <c r="T5" t="inlineStr">
+      <c r="V5" t="inlineStr">
         <is>
           <t>['310', 'No', 'Yes', 'n/a']</t>
         </is>
@@ -742,35 +783,35 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>int</t>
         </is>
       </c>
       <c r="D6" t="n">
         <v>3335</v>
       </c>
       <c r="E6" t="n">
-        <v>3335</v>
+        <v>3311</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>147322</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>44.49471458773785</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>14.46911135959427</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>209.35518353634</v>
       </c>
       <c r="K6" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="L6" t="n">
-        <v>-1</v>
+        <v>88</v>
       </c>
       <c r="M6" t="n">
         <v>0</v>
@@ -784,18 +825,26 @@
       <c r="P6" t="n">
         <v>4</v>
       </c>
-      <c r="Q6" t="inlineStr">
+      <c r="Q6" t="n">
+        <v>18</v>
+      </c>
+      <c r="R6" t="inlineStr">
         <is>
           <t>n/a</t>
         </is>
       </c>
-      <c r="R6" t="n">
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="T6" t="n">
         <v>6575</v>
       </c>
-      <c r="S6" t="n">
+      <c r="U6" t="n">
         <v>88</v>
       </c>
-      <c r="T6" t="inlineStr">
+      <c r="V6" t="inlineStr">
         <is>
           <t>['1', '10', '11', '12', '13', '14', '15', '16', '17', '18', '19', '2', '20', '21', '22', '23', '24', '25', '26', '27', '28', '29', '3', '3.5', '30', '31', '32', '33', '34', '35', '36', '37', '38', '39', '4', '4.5', '40', '41', '42', '43', '44', '45', '46', '47', '48', '49', '5', '50', '51', '52', '53', '54', '55', '56', '57', '58', '59', '6', '60', '61', '62', '63', '64', '65', '66', '67', '68', '69', '7', '70', '71', '72', '73', '74', '75', '76', '77', '78', '79', '8', '80', '82', '83', '84', '86', '88', '9', 'n/a']</t>
         </is>
@@ -854,18 +903,26 @@
       <c r="P7" t="n">
         <v>4</v>
       </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="R7" t="n">
+      <c r="Q7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>Labourer</t>
+        </is>
+      </c>
+      <c r="T7" t="n">
         <v>26327</v>
       </c>
-      <c r="S7" t="n">
+      <c r="U7" t="n">
         <v>120</v>
       </c>
-      <c r="T7" t="inlineStr">
+      <c r="V7" t="inlineStr">
         <is>
           <t>['182', 'Accountant', 'Agent', 'Baker', 'Barber', 'Blacksmith', 'Boarding housekeeper', 'Book keeper', 'Bookkeeper', 'Butcher', 'Cabinet maker', 'Camel driver', 'Camp cook', 'Caretaker', 'Caretaker Joss House', 'Carpenter', 'Carrier', 'Carter', 'Chinese Minister', 'Chinese Storekeeper', 'Church', 'Clerk', 'Contractor', 'Cook', 'Cook and Carpenter', 'Cook and Gardener', 'Cycle and Motor Car Agent', 'Dairy hand', 'Diver', 'Domestic', 'Domestic duties', 'Domestic servant', 'Draper', 'Dressmaker', 'Engine Driver', 'Engineer', 'Farm hand', 'Farm work', 'Farmer', 'Fisher man', 'Fisherman', 'Fishmonger', 'Fossicker', 'Fowl dealer', 'Fruit and Vegetable hawker', 'Fruit hawker', 'Fruiter', 'Fruiterer', 'Fruiterer and Confection', 'Fruiterer and Green grocer', 'Ganger', 'Garden labourer', 'Gardener', 'Gem buyer', 'General storekeeper', 'Grazier', 'Green Grocer and Fruiterer', 'Greengrocer', 'Grocer', 'Hawker', 'Home duties', 'Home duty', 'Horsebreaker', 'House duties', 'House keeper Joss', 'Household', 'Household duties', 'Housekeeper', 'Housewife', 'Housework', 'Jeweller', 'Keeper of refreshment rooms', 'Labourer', 'Laundry man', 'Laundry proprietor', 'Laundry-man', 'Laundryman', 'Licensed Victualler and Storekeeper', 'Manager', 'Market gardener', 'Merchant', 'Milliner', 'Miner', 'Motor Car Driver', 'Overseer', 'Pensioner', 'Porter', 'Poultry farmer', 'Produce hawker', 'Prospector', 'Prostitute', 'Refreshment room', 'Restaurant keeper', 'Salesman', 'Scalper', 'Selector', 'Selector and Bootmaker', 'Servant', 'Shop assistant', 'Shopkeeper', 'Slaughterman', 'Station cook', 'Station hand', 'Stockman', 'Storekeeper', 'Storekeeper and Baker', 'Storekeeper and Hawker', 'Storeman', 'Tailor', 'Teacher', 'Tin miner', 'Tin miner and Gardener', 'Tobacco grower', 'Upholsterer', 'Vegetable gardener', 'Vegetable hawker', 'Waiter', 'Worker', 'labourer', 'n/a']</t>
         </is>
@@ -924,18 +981,26 @@
       <c r="P8" t="n">
         <v>3</v>
       </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>na</t>
-        </is>
-      </c>
-      <c r="R8" t="n">
+      <c r="Q8" t="n">
+        <v>312</v>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="T8" t="n">
         <v>12993</v>
       </c>
-      <c r="S8" t="n">
+      <c r="U8" t="n">
         <v>67</v>
       </c>
-      <c r="T8" t="inlineStr">
+      <c r="V8" t="inlineStr">
         <is>
           <t>['10', '1833', '1850', '1852', '1853', '1856', '1857', '1859', '1860', '1861', '1862', '1863', '1864', '1865', '1866', '1867', '1868', '1869', '1870', '1871', '1872', '1873', '1874', '1875', '1876', '1877', '1878', '1879', '1880', '1881', '1882', '1883', '1884', '1885', '1886', '1887', '1888', '1889', '1890', '1891', '1892', '1893', '1894', '1895', '1896', '1897', '1898', '1899', '1900', '1901', '1902', '1903', '1904', '1905', '1906', '1907', '1908', '1909', '1910', '1911', '1912', '1913', '1998', '1999', '312', 'n/a', 'na']</t>
         </is>
@@ -994,18 +1059,26 @@
       <c r="P9" t="n">
         <v>4</v>
       </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="R9" t="n">
+      <c r="Q9" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>Mackay</t>
+        </is>
+      </c>
+      <c r="T9" t="n">
         <v>34383</v>
       </c>
-      <c r="S9" t="n">
+      <c r="U9" t="n">
         <v>446</v>
       </c>
-      <c r="T9" t="inlineStr">
+      <c r="V9" t="inlineStr">
         <is>
           <t>['25', 'Aberdeen', 'Aberdeen C', 'Aberdeen Creek', 'Abingdon Downs', 'Aitkenvale', 'Alabama Flat', 'Albert Street Warwick', 'Albert and Denison Streets Rockhampton', 'Albion Street Warwick', 'Allora', 'Alma Lane', 'Alma Street', 'Alpha', 'Ambo', 'Amby', 'Angore', 'Annandale', 'Apsey Farm Inglewood', 'Archer Street', 'Augustus Downs', 'Aurora Creek', 'Ayr', 'Babo', 'Bakers Creek', 'Balaclava Street', 'Balangowan', 'Ballandean', 'Balnagowan', 'Banana', 'Barfield Station Banana', 'Bath Farm Omanama', 'Bell', 'Bellagammon', 'Belmore', 'Benaraby', 'Black Creek Englands Pocket', 'Black Ridge', 'Blackbutt', 'Blue Mountain Stanthorpe', 'Bluff Road', 'Bollon', 'Bolsover St Rockhampton', 'Bolsover Street', 'Bolsover Street Rockhampton', 'Bolsover and Cambridge Streets', 'Bolsover and Wood Streets Rockhampton', 'Borella', 'Bowen', 'Boyne Island', 'Brandon', 'Brisbane Claim Stanthorpe', 'Brisbane Street', 'Brisk St', 'Brisk Street', 'Brookdale', 'Brookfield Farm Inglewood', 'Brookland', 'Brooks Creek', 'Broughton', 'Bungil Creek Roma', 'Bungil St Roma', 'Bungil Street Roma', 'Burketown', 'Caley Valley', 'Calliope', 'Cambooya', 'Campbell and Albert Streets Rockhampton', 'Campbell and Archer Street', 'Cania', 'Canning Creek Station Inglewood', 'Canning Park Inglewood', 'Cape River', 'Capella', 'Cardigan', 'Carpentaria', 'Carron River', 'Catfishfish Creek Inglewood', 'Cemetry Road Mount Morgan', 'Central Street Mount Morgan', 'Charters Towers', 'Charters Towers Road', 'Ching Do', 'Christmas Creek', 'Clarina', 'Clarks Farm Inglewood', 'Clermont', 'Clermont Street Emerald', 'Cleveland', 'Clifton', 'Club Hotel', 'Cobvale', 'Colevale', 'Comootoo Caroo Station', 'Condamine Killarney', 'Condamine Plains Station', 'Coomrith', 'Coorooman', 'Cork Creek', 'Corner Denison and Derby Streets Rockhampton', 'Cowan Downs', 'Cr Denison and Derby Streets Rockhampton', 'Criterion Hotel', 'Crown Hotel', 'Croxley Kingsthorpe', 'Croydon', 'Cumberland', 'Dalby', 'Dalcooth Stanthorpe', 'Dareel Station Mungindi', 'Dareel Stn Mungindi', 'Deane Street', 'Dearies C', 'Dearies Creek', 'Dee Rush Mount Morgan', 'Dee Track Mount Morgan', 'Denham Street', 'Denison Lane Rockhampton', 'Denison Street Rockhampton', 'Derby Street', 'Deuchars Creek', 'Dexter Street', 'Don Delta', 'Donors Hills', 'Dumbleton', 'Dunbar', 'Durham', 'East Street', 'East Street Mount Morgan', 'East Swamp', 'Eddington Street', 'Egerah Station', 'Egilabria', 'Einasleigh', 'Ellangowan', 'Elphinstone Lane', 'Elphinstone Street', 'Emerald', 'Emu Park', 'Emu Park Hotel', 'Emu Vale', 'Escott', 'Eyre Street', 'Fairfield', 'Fairfield Station', 'Fairleigh', 'Farleigh', 'Fiery Downs', 'Finch Hatton', 'Fitzroy Street', 'Fitzroy Street Warwick', 'Fitzroy and Talford Streets', 'Flinders Street', 'Ford Street', 'Forest Hill', 'Forest Home', 'Forsayth', 'Four Mile Creek', 'Gards Lane', 'Gatton', 'George Street Roma', 'Georgetown', 'German Gardens', 'Gill St', 'Gill Street', 'Gladstone', 'Gladstone Creek', 'Gladstone Street', 'Glassford Creek', 'Glenearn Surat', 'Glenmore', 'Glenmore Road', 'Glenore', 'Golden Gate', 'Goodurus Farm Inglewood', 'Goodwin Farm Inglewood', 'Goombungee', 'Goondiwindi', 'Grafton Street Warwick', 'Grand Hotel', 'Grand Hotel Emerald', 'Green Hills Station', 'Greenvale', 'Gregory Downs', 'Gregory St Roma', 'Gregory Street Roma', 'Grey Street Warwick', 'Grosvenor Downs', "Gunn's Farm off Forest Road Laidley", 'Gunns Farm', 'Gunns Paddock off Forest Hill Road', 'Gunyan Station', 'Habana', 'Halifax', 'Hantley Street Warwick', 'Happy Valley', 'Hebel', 'High St', 'High Street', 'Hillgrove', 'Hills Farm Inglewood', 'Homebush', 'Homestead', 'Horse Creek Mount Morgan', 'Hospital', 'Huntly Station', 'Hyde Park', 'Iffley', 'Ingham', 'Inglewood', 'Inverleigh', 'Island Station', 'James Street', 'Jinghi Creek Jandowaie', 'Kalamia', 'Kalka', 'Kalka Street', 'Keepkie Farm Nine Mile', 'Kelvin Grove', 'Kent Street', 'Kidston', 'Killarney', 'Kings Creek', 'Kingumbilla', 'Kirk Dgs', 'Kondar', 'Koongal', 'Kurrowah Station', 'Kyoomba Stanthorpe', 'Lamberts Crossing', 'Lassie Creek', 'Lawn Hills', 'Leyburn', 'Limevale', 'Lion Creek', 'Little Street', 'Lochinvar', 'Lorraine', 'Lotus Creek', 'Louie Creek', 'Louie Creek Garden', 'Lovells Farm Inglewood', 'Lower East Street Rockhampton', 'Lowstaff Capella', 'Lyndhurst Warwick', 'Mackay', 'Macknade', 'Maggieville', 'Magoura', 'Maidavale', 'Margaret Street', 'Market Garden', 'McKenzie Street', 'Melrose Killarney', 'Middle Ridge', 'Mile Creek Toonda', 'Miles', 'Mill Hill Warwick', 'Millchester', 'Mimosa Vale Station Banana', 'Minil', 'Mirani', 'Mitchell', 'Moore Street', 'Morgan Street Mount Morgan', 'Mosman Park', 'Mosman Pk', 'Mosman Street', 'Mount Chalmers', 'Mount Jukes', 'Mount Sturt', 'Mount Surprise', 'Mount Vince', 'Mt Abundance Roma', 'Mt Brown', 'Mt Jukes', 'Mt Larcom', 'Mt Vince', 'Muckadilla Hotel', 'Mungindi', 'Murry River', 'Musgrave Street', 'Nabia', 'Nankin Creek', 'Narine Station Mungindi', 'National Hotel', 'Nebia', 'Nebo', 'Neumayer Valley', 'Newbury', 'Newinga Mungindi', 'Noondoo Run Mungindi', 'Noondoo St Thallon', 'Noondoo Street Thallon', 'Normanton', 'Nutgrove', 'O Briens Creek', 'Oakey Creek Oakey', 'Palmerin Street Warwick', 'Palms Est.', 'Palms Estuary', 'Park Avenue', 'Parsons Point', 'Pentland', 'Pimlico', 'Pinfield', 'Pink Lily', 'Pioneer', 'Pioneer Orchard', 'Plane Ck', 'Plane Creek', 'Port Curtis Road', 'Pratten', 'Proserpine', 'Prospect', 'Punjab', "Q'lander.C.", 'Queens Hotel', 'Queens Park', 'Queensland', 'Queenslander C', "R'wood", 'Raglan Creek', 'Raglan Station', 'Ravenswood', 'Ravenswood Junction', 'Reids Garden', 'Retro Station Capella', 'Ripple Ck', 'Ripple Creek', 'Rising Sun Garden', 'Rising Sun Hotel Warra', 'Riverside', 'Riversleigh', 'Rockford', 'Rockhampton', 'Rodds Bay', 'Rolleston', 'Roma', 'Rookwood Surat', 'Rose Bay', 'Rosebank', 'Rosella Plains', 'Ross Creek', 'Ross River', 'Royal Hotel', 'Ruby Ridge', 'Russell Street', 'Ruthven Street', "S. T'ville", 'Saltbush Park', 'Sandhills', 'Sandy Creek', 'Sapphire', 'Sarina', 'Savannah', 'Scrubby Creek', 'Sea View Hotel', 'Sellheim', 'Seymour River', 'Silverspur', 'Sir Street', 'South St Rockhampton', 'South Street', 'South Townsville', 'South and Bolsover Streets Rockhampton', 'Spring Creek', 'Springsure', 'Spung Creek', 'St George', 'Stanley St Rockhampton', 'Stanley and Bolsover Streets Rockhampton', 'Stanley and Bolsover Sts Rockhampton', 'Stanley and Murray Streets Rockhampton', 'Stanley and Murray Streetss Rockhampton', 'Stanthorpe', 'Stanthorpe Blue Mountain', 'Station Creek', 'Stephen Street', 'Sterling', 'Stewart Street', 'Stewarts C', 'Stoke St', 'Stoke Street', 'Stone River', 'Strathmore', 'Struck Oil Mount Morgan', 'Sugar Mill Yeppoon', 'Sugarloaf', 'Sugarloaf Stanthorpe', 'Surat', 'Tabletop Creek', 'Tanby', 'Telemon', 'Texas', 'Texas Flat', 'Texas Station', 'The Island Cobba-da-mana', 'The Leap', 'The Ridge', 'The Ridges', 'Three Mile', 'Toolbuna Warwick', 'Toolooa', 'Toonda', 'Townsville', 'Tully River', 'Turn Off Lagoon', 'Upper Dee Mt Morgan', 'Upper Dee River Mount Morgan', 'Vanrook', 'Venur', 'Victoria Downs Station', 'Victoria Street Forest Hill', 'Walkerston', 'Warra', 'Warradinga', 'Warwick', 'Water Street', 'Waverley', 'Wayworth', 'Weribone Street Surat', 'West End', 'West Street', 'Western Creek', 'Westmoreland', 'Westwood', 'Wild Bull Gully Mount', 'William Street', 'Willowburn', 'Wombull', 'Wondoola', 'Wood St', 'Wood Street', 'Wormyvilla', 'Yacamunda', 'Yalebone Creek Roma', 'Yandilla Station', 'Yarran Dns Surat', 'Yarran Downs Surat', 'Yarwan', 'Yeppoon', 'Yeulba', 'Yingerbay via Roma', 'Yogango Estate Yogango', 'n/a']</t>
         </is>
@@ -1064,18 +1137,26 @@
       <c r="P10" t="n">
         <v>5</v>
       </c>
-      <c r="Q10" t="inlineStr">
+      <c r="Q10" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
         <is>
           <t>Townsville</t>
         </is>
       </c>
-      <c r="R10" t="n">
+      <c r="T10" t="n">
         <v>31606</v>
       </c>
-      <c r="S10" t="n">
+      <c r="U10" t="n">
         <v>5</v>
       </c>
-      <c r="T10" t="inlineStr">
+      <c r="V10" t="inlineStr">
         <is>
           <t>['Normanton', 'Rockhampton', 'Roma', 'Toowoomba', 'Townsville']</t>
         </is>
@@ -1134,18 +1215,26 @@
       <c r="P11" t="n">
         <v>4</v>
       </c>
-      <c r="Q11" t="inlineStr">
+      <c r="Q11" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
         <is>
           <t>n/a</t>
         </is>
       </c>
-      <c r="R11" t="n">
+      <c r="T11" t="n">
         <v>28428</v>
       </c>
-      <c r="S11" t="n">
+      <c r="U11" t="n">
         <v>104</v>
       </c>
-      <c r="T11" t="inlineStr">
+      <c r="V11" t="inlineStr">
         <is>
           <t>['356', 'Allenstown', 'Allora', 'Alma Street', 'Alpha', 'Ayr', 'Banana', 'Bowen', 'Brandon', 'Burketown', 'Calliope', 'Cambooya', 'Capella', 'Cardwell', 'Charters Towers', 'Clarke River', 'Clermont', 'Clifton', 'Cooyar', 'Croydon', 'Cumberland', 'Dalby', 'Duarunga', 'Einasleigh', 'Emerald', 'Emu Park', 'Eton Mackay', 'Ewan', 'Farleigh Mackay', 'Finch Hatton', 'Forest Hill', 'Forsayth', 'Gatton', 'Georgetown', 'Gilbert River', 'Goombungee', 'Goondiwindi', 'Gregory Downs', 'Halifax', 'Homebush', 'Ingham', 'Inglewood', 'Jandowaie', 'Killarney', 'Kingsthorpe', 'Laidley', 'Lakes Creek', 'Leyburn', 'Liontown', 'Mackay', 'Many Peaks', 'Marian Mackay', 'Marmor', 'Merinda', 'Middle Ridge', 'Millchester', 'Millmerran', 'Mirani Mackay', 'Mount Morgan', 'Mount Surprise', 'Mt Chalmers', 'Mt Morgan', 'Mt Surprise', 'Mundingburra', 'Nebo Mackay', 'Normanton', 'North Rockhampton', 'North Ward', 'Oakey', 'Oaks', 'Pentland', 'Pratten', 'Proserpine', 'Queenton', 'Ravenswood', 'Ravenswood Junction', 'Rockhampton', 'Rolleston', 'Sadds Ridge', 'Sapphire', 'Sarina  Mackay', 'Sarina Mackay', 'Sellheim', 'Seymour River', 'Silverspur', 'South Townsville', 'Springsure', 'St Laurence', 'Stanthorpe', 'Stewarts Creek', 'Texas', 'Toowoomba', 'Townsville', 'Turn Off Lagoons', 'Ukalunda', 'Walkerston  Mackay', 'Walkerston Mackay', 'Warra', 'Warwick', 'West End', 'Westwood', 'Yangan', 'Yeppoon', 'n/a']</t>
         </is>

</xml_diff>